<commit_message>
Fix bugs and test
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/full_6.xlsx
+++ b/tests/integration_test_files/full_6.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88483F36-1C0F-AC48-8B31-2960CE8C7082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEFB608B-82CB-BE4B-A02D-3C776FBBBDB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="61680" yWindow="500" windowWidth="37880" windowHeight="23700" firstSheet="18" activeTab="26" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="61680" yWindow="500" windowWidth="37880" windowHeight="23700" firstSheet="18" activeTab="27" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3337" uniqueCount="1268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3338" uniqueCount="1269">
   <si>
     <t>name</t>
   </si>
@@ -3876,6 +3876,9 @@
   </si>
   <si>
     <t>masking</t>
+  </si>
+  <si>
+    <t>Investigator</t>
   </si>
 </sst>
 </file>
@@ -14098,8 +14101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B62A79FA-4693-DC4C-8533-78F85FC1D1D4}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14149,7 +14152,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54F6DEFA-A517-8846-A522-4BE1FE1D8CBC}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -14188,6 +14191,9 @@
       </c>
       <c r="D2" t="s">
         <v>1266</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1268</v>
       </c>
     </row>
   </sheetData>

</xml_diff>